<commit_message>
Update 2023 06 (june) 06
</commit_message>
<xml_diff>
--- a/readme-code-details.xlsx
+++ b/readme-code-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karan\Documents\Racing\greyhound-racing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BC8909-2594-45E9-858B-AADFFEF1FEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2081F577-822C-4212-AAC2-722A39E2EC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Codename</t>
   </si>
@@ -141,6 +141,21 @@
 a) 5 X dog_results_....csv
 b) 5 X race_details_....csv
 c) doggradeinfo_....csv
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C020_FT Dataprep_Base.ipynb
+</t>
+  </si>
+  <si>
+    <t>raw_base_2023-06-05.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Takes the raw data and adds :
+a) winner, top3, measurement for random 
+b) winner, top3, measurement for fast-track cols 
+then filters for the created columns and exports. 
+Measurement variable include (hits, profitability for winner, all place to wins, lay last)
 </t>
   </si>
 </sst>
@@ -200,19 +215,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -498,7 +509,7 @@
   <dimension ref="C3:H19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,22 +523,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -538,12 +549,12 @@
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="3"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
@@ -552,12 +563,12 @@
       <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="3:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
@@ -566,16 +577,16 @@
       <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="3"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="3:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
@@ -584,16 +595,16 @@
       <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -604,23 +615,31 @@
       <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C9" s="2"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+    <row r="9" spans="3:8" ht="144" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
CGPT updates 2023 06 07
</commit_message>
<xml_diff>
--- a/readme-code-details.xlsx
+++ b/readme-code-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karan\Documents\Racing\greyhound-racing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2081F577-822C-4212-AAC2-722A39E2EC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED4CD4F-2472-4629-B087-43545D34D449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Codename</t>
   </si>
@@ -156,6 +156,17 @@
 b) winner, top3, measurement for fast-track cols 
 then filters for the created columns and exports. 
 Measurement variable include (hits, profitability for winner, all place to wins, lay last)
+</t>
+  </si>
+  <si>
+    <t>C021_FT Dataprep_Speed Profile.ipynb</t>
+  </si>
+  <si>
+    <t>f'dataprep_speed_profile_{todaydt}.csv'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create speed profile variables such as 
+distance total, distance group, race time group etc
 </t>
   </si>
 </sst>
@@ -180,12 +191,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -215,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -225,6 +242,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,14 +528,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF0E014-B602-40D6-9131-260E11F53161}">
   <dimension ref="C3:H19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="4.44140625" customWidth="1"/>
-    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="40.33203125" customWidth="1"/>
     <col min="7" max="7" width="47.21875" customWidth="1"/>
@@ -523,22 +543,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -642,12 +662,22 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+    <row r="10" spans="3:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.3">

</xml_diff>